<commit_message>
Jupyter Notebook to Download ETF Holdings from ETFDb Added
</commit_message>
<xml_diff>
--- a/Major 4 Etfs.xlsx
+++ b/Major 4 Etfs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kshitizsharma/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kshitizsharma/Desktop/ETFAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9931460-23C7-EF42-980E-869AD5C7D9B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F0053E-381A-E847-AB52-964E89E7CEB4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16220" xr2:uid="{243AC440-5425-EE4B-AD5A-AECD16926CB5}"/>
   </bookViews>
@@ -20,11 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -68,9 +63,6 @@
     <t>VGT</t>
   </si>
   <si>
-    <t>FETC</t>
-  </si>
-  <si>
     <t>IYE</t>
   </si>
   <si>
@@ -120,6 +112,9 @@
   </si>
   <si>
     <t>FHLC</t>
+  </si>
+  <si>
+    <t>FTEC</t>
   </si>
 </sst>
 </file>
@@ -484,7 +479,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -527,7 +522,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -541,61 +536,61 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
         <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
         <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>